<commit_message>
[OPT-3] - Small test file fix
</commit_message>
<xml_diff>
--- a/OPTEL.UI.Desktop.Test/Assets/MariaSoelUploadDataTest.xlsx
+++ b/OPTEL.UI.Desktop.Test/Assets/MariaSoelUploadDataTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MS Visual Studio 2019\OPTEL\OPTEL.UI.Desktop.Test\bin\Debug\netcoreapp3.1\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MS Visual Studio 2019\OPTEL\OPTEL.UI.Desktop.Test\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4207804B-605B-48EA-B418-61BD762CBF09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1031EF-172B-4358-8CC8-81773534CE3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3F964C94-F0DC-451B-9B82-1F291A0CA648}"/>
   </bookViews>
@@ -6515,8 +6515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA776DB7-E681-4B90-8897-81C1B21273F9}">
   <dimension ref="A1:G319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7078,7 +7078,7 @@
         <v>15.1</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>